<commit_message>
minor update to the results
</commit_message>
<xml_diff>
--- a/results/bulk_performance.xlsx
+++ b/results/bulk_performance.xlsx
@@ -52,7 +52,7 @@
     <t>1:10.86</t>
   </si>
   <si>
-    <t>00:01:10</t>
+    <t>00:00:54</t>
   </si>
   <si>
     <t>debga</t>
@@ -79,7 +79,7 @@
     <t>1:31.38</t>
   </si>
   <si>
-    <t>00:01:31</t>
+    <t>00:01:17</t>
   </si>
   <si>
     <t>1:10.12</t>
@@ -100,7 +100,7 @@
     <t>0:37.81</t>
   </si>
   <si>
-    <t>00:00:37</t>
+    <t>00:00:19</t>
   </si>
   <si>
     <t>1:09.56</t>
@@ -121,7 +121,7 @@
     <t>5:31.41</t>
   </si>
   <si>
-    <t>00:05:32</t>
+    <t>00:05:17</t>
   </si>
   <si>
     <t>2:52.80</t>
@@ -139,7 +139,7 @@
     <t>7:36.44</t>
   </si>
   <si>
-    <t>00:07:37</t>
+    <t>00:07:22</t>
   </si>
   <si>
     <t>2:59.26</t>
@@ -157,7 +157,7 @@
     <t>1:59.36</t>
   </si>
   <si>
-    <t>00:01:59</t>
+    <t>00:01:45</t>
   </si>
   <si>
     <t>2:43.95</t>
@@ -178,7 +178,7 @@
     <t>2:33.94</t>
   </si>
   <si>
-    <t>00:02:34</t>
+    <t>00:02:20</t>
   </si>
   <si>
     <t>1:16.40</t>
@@ -196,7 +196,7 @@
     <t>4:59.97</t>
   </si>
   <si>
-    <t>00:05:00</t>
+    <t>00:04:45</t>
   </si>
   <si>
     <t>1:15.07</t>
@@ -214,6 +214,9 @@
     <t>0:36.51</t>
   </si>
   <si>
+    <t>00:00:22</t>
+  </si>
+  <si>
     <t>1:12.15</t>
   </si>
   <si>
@@ -232,7 +235,7 @@
     <t>1:10.15</t>
   </si>
   <si>
-    <t>00:01:09</t>
+    <t>00:00:55</t>
   </si>
   <si>
     <t>1:12.12</t>
@@ -250,7 +253,7 @@
     <t>1:34.22</t>
   </si>
   <si>
-    <t>00:01:34</t>
+    <t>00:01:20</t>
   </si>
   <si>
     <t>1:12.54</t>
@@ -268,7 +271,7 @@
     <t>0:35.83</t>
   </si>
   <si>
-    <t>00:00:35</t>
+    <t>00:00:17</t>
   </si>
   <si>
     <t>1:07.45</t>
@@ -286,7 +289,7 @@
     <t>5:38.30</t>
   </si>
   <si>
-    <t>00:05:37</t>
+    <t>00:05:22</t>
   </si>
   <si>
     <t>2:56.73</t>
@@ -304,7 +307,7 @@
     <t>7:42.04</t>
   </si>
   <si>
-    <t>00:07:41</t>
+    <t>00:07:25</t>
   </si>
   <si>
     <t>3:02.68</t>
@@ -322,9 +325,6 @@
     <t>2:04.11</t>
   </si>
   <si>
-    <t>00:02:03</t>
-  </si>
-  <si>
     <t>2:49.81</t>
   </si>
   <si>
@@ -340,7 +340,7 @@
     <t>2:40.87</t>
   </si>
   <si>
-    <t>00:02:40</t>
+    <t>00:02:22</t>
   </si>
   <si>
     <t>1:14.46</t>
@@ -358,7 +358,7 @@
     <t>5:00.18</t>
   </si>
   <si>
-    <t>00:04:59</t>
+    <t>00:04:44</t>
   </si>
   <si>
     <t>1:20.50</t>
@@ -376,7 +376,7 @@
     <t>0:38.43</t>
   </si>
   <si>
-    <t>00:00:38</t>
+    <t>00:00:24</t>
   </si>
   <si>
     <t>1:12.46</t>
@@ -1216,7 +1216,7 @@
         <v>65</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1230,10 +1230,10 @@
         <v>64.23</v>
       </c>
       <c r="F27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1247,15 +1247,15 @@
         <v>28.39</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>8</v>
@@ -1270,10 +1270,10 @@
         <v>19.81</v>
       </c>
       <c r="F29" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1287,10 +1287,10 @@
         <v>64.26000000000001</v>
       </c>
       <c r="F30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1304,10 +1304,10 @@
         <v>27.68</v>
       </c>
       <c r="F31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1323,10 +1323,10 @@
         <v>20.21</v>
       </c>
       <c r="F32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1340,10 +1340,10 @@
         <v>64.56999999999999</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1357,10 +1357,10 @@
         <v>27.72</v>
       </c>
       <c r="F34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1376,10 +1376,10 @@
         <v>19.73</v>
       </c>
       <c r="F35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1393,10 +1393,10 @@
         <v>64.48999999999999</v>
       </c>
       <c r="F36" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1410,10 +1410,10 @@
         <v>27.74</v>
       </c>
       <c r="F37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1431,10 +1431,10 @@
         <v>19.82</v>
       </c>
       <c r="F38" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1448,10 +1448,10 @@
         <v>64.29000000000001</v>
       </c>
       <c r="F39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G39" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1465,10 +1465,10 @@
         <v>27.99</v>
       </c>
       <c r="F40" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G40" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1484,10 +1484,10 @@
         <v>20.23</v>
       </c>
       <c r="F41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1501,10 +1501,10 @@
         <v>64.29000000000001</v>
       </c>
       <c r="F42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G42" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1518,10 +1518,10 @@
         <v>27.98</v>
       </c>
       <c r="F43" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1537,10 +1537,10 @@
         <v>19.74</v>
       </c>
       <c r="F44" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:7">

</xml_diff>